<commit_message>
form2Excel >> javadoc added, excelMM_template レイアウト調整
</commit_message>
<xml_diff>
--- a/GoodSunLMS/src/main/java/com/reality/util/excel/ExcelMM_template.xlsx
+++ b/GoodSunLMS/src/main/java/com/reality/util/excel/ExcelMM_template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8C8BD6-6C39-4173-B5E0-E3DDCF81DCEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51CCC0A-694E-45F0-9F3C-5E6F7B695D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22015" yWindow="-104" windowWidth="22325" windowHeight="11924" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="230" yWindow="1110" windowWidth="14400" windowHeight="9430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -143,12 +143,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="176" formatCode="yyyy&quot;年&quot;mm&quot;月度&quot;"/>
     <numFmt numFmtId="177" formatCode="mm/dd"/>
     <numFmt numFmtId="178" formatCode="aaa"/>
     <numFmt numFmtId="179" formatCode="[h]:mm"/>
-    <numFmt numFmtId="180" formatCode="h:mm"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -507,7 +506,7 @@
     <xf numFmtId="178" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -528,26 +527,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -567,9 +566,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -607,9 +606,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -642,26 +641,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -694,26 +676,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -890,12 +855,22 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="I3" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.08984375" customWidth="1"/>
+    <col min="2" max="2" width="3.6328125" customWidth="1"/>
+    <col min="3" max="4" width="7" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="6" max="6" width="9.08984375" customWidth="1"/>
+    <col min="7" max="7" width="13.26953125" customWidth="1"/>
+    <col min="8" max="8" width="10.6328125" customWidth="1"/>
+    <col min="9" max="9" width="22.6328125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.850000000000001" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
@@ -908,20 +883,20 @@
       <c r="H1" s="26"/>
       <c r="I1" s="27"/>
     </row>
-    <row r="2" spans="1:9" ht="17.850000000000001" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="32"/>
+    <row r="2" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="30"/>
       <c r="G2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="33"/>
-      <c r="I2" s="34"/>
-    </row>
-    <row r="3" spans="1:9" ht="17.850000000000001" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="31"/>
+      <c r="I2" s="32"/>
+    </row>
+    <row r="3" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="3"/>
       <c r="C3" s="1"/>
@@ -932,11 +907,11 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="17.850000000000001" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+    <row r="4" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="29"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="12" t="s">
         <v>3</v>
       </c>
@@ -959,7 +934,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="17.3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" s="21"/>
@@ -970,7 +945,7 @@
       <c r="H5" s="10"/>
       <c r="I5" s="9"/>
     </row>
-    <row r="6" spans="1:9" ht="17.3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
       <c r="A6" s="22"/>
       <c r="B6" s="23"/>
       <c r="C6" s="21"/>
@@ -981,7 +956,7 @@
       <c r="H6" s="10"/>
       <c r="I6" s="9"/>
     </row>
-    <row r="7" spans="1:9" ht="17.3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
       <c r="A7" s="22"/>
       <c r="B7" s="23"/>
       <c r="C7" s="21"/>
@@ -992,7 +967,7 @@
       <c r="H7" s="10"/>
       <c r="I7" s="9"/>
     </row>
-    <row r="8" spans="1:9" ht="17.3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="21"/>
@@ -1003,7 +978,7 @@
       <c r="H8" s="10"/>
       <c r="I8" s="9"/>
     </row>
-    <row r="9" spans="1:9" ht="17.3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="21"/>
@@ -1014,7 +989,7 @@
       <c r="H9" s="10"/>
       <c r="I9" s="9"/>
     </row>
-    <row r="10" spans="1:9" ht="17.3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="21"/>
@@ -1025,7 +1000,7 @@
       <c r="H10" s="10"/>
       <c r="I10" s="9"/>
     </row>
-    <row r="11" spans="1:9" ht="17.3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="21"/>
@@ -1036,7 +1011,7 @@
       <c r="H11" s="10"/>
       <c r="I11" s="9"/>
     </row>
-    <row r="12" spans="1:9" ht="17.3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="21"/>
@@ -1047,7 +1022,7 @@
       <c r="H12" s="10"/>
       <c r="I12" s="9"/>
     </row>
-    <row r="13" spans="1:9" ht="17.3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
       <c r="A13" s="22"/>
       <c r="B13" s="23"/>
       <c r="C13" s="21"/>
@@ -1058,7 +1033,7 @@
       <c r="H13" s="10"/>
       <c r="I13" s="9"/>
     </row>
-    <row r="14" spans="1:9" ht="17.3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
       <c r="A14" s="22"/>
       <c r="B14" s="23"/>
       <c r="C14" s="21"/>
@@ -1069,7 +1044,7 @@
       <c r="H14" s="10"/>
       <c r="I14" s="9"/>
     </row>
-    <row r="15" spans="1:9" ht="17.3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
       <c r="A15" s="22"/>
       <c r="B15" s="23"/>
       <c r="C15" s="21"/>
@@ -1080,7 +1055,7 @@
       <c r="H15" s="10"/>
       <c r="I15" s="9"/>
     </row>
-    <row r="16" spans="1:9" ht="17.3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
       <c r="A16" s="22"/>
       <c r="B16" s="23"/>
       <c r="C16" s="21"/>
@@ -1091,7 +1066,7 @@
       <c r="H16" s="10"/>
       <c r="I16" s="9"/>
     </row>
-    <row r="17" spans="1:9" ht="17.3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
       <c r="A17" s="22"/>
       <c r="B17" s="23"/>
       <c r="C17" s="21"/>
@@ -1102,7 +1077,7 @@
       <c r="H17" s="10"/>
       <c r="I17" s="9"/>
     </row>
-    <row r="18" spans="1:9" ht="17.3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
       <c r="A18" s="22"/>
       <c r="B18" s="23"/>
       <c r="C18" s="21"/>
@@ -1113,7 +1088,7 @@
       <c r="H18" s="10"/>
       <c r="I18" s="9"/>
     </row>
-    <row r="19" spans="1:9" ht="17.3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
       <c r="A19" s="22"/>
       <c r="B19" s="23"/>
       <c r="C19" s="21"/>
@@ -1124,7 +1099,7 @@
       <c r="H19" s="10"/>
       <c r="I19" s="9"/>
     </row>
-    <row r="20" spans="1:9" ht="17.3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
       <c r="A20" s="22"/>
       <c r="B20" s="23"/>
       <c r="C20" s="21"/>
@@ -1135,7 +1110,7 @@
       <c r="H20" s="10"/>
       <c r="I20" s="9"/>
     </row>
-    <row r="21" spans="1:9" ht="17.3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
       <c r="A21" s="22"/>
       <c r="B21" s="23"/>
       <c r="C21" s="21"/>
@@ -1146,7 +1121,7 @@
       <c r="H21" s="10"/>
       <c r="I21" s="9"/>
     </row>
-    <row r="22" spans="1:9" ht="17.3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
       <c r="A22" s="22"/>
       <c r="B22" s="23"/>
       <c r="C22" s="21"/>
@@ -1157,7 +1132,7 @@
       <c r="H22" s="10"/>
       <c r="I22" s="9"/>
     </row>
-    <row r="23" spans="1:9" ht="17.3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
       <c r="A23" s="22"/>
       <c r="B23" s="23"/>
       <c r="C23" s="21"/>
@@ -1168,7 +1143,7 @@
       <c r="H23" s="10"/>
       <c r="I23" s="9"/>
     </row>
-    <row r="24" spans="1:9" ht="17.3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
       <c r="A24" s="22"/>
       <c r="B24" s="23"/>
       <c r="C24" s="21"/>
@@ -1179,7 +1154,7 @@
       <c r="H24" s="10"/>
       <c r="I24" s="9"/>
     </row>
-    <row r="25" spans="1:9" ht="17.3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
       <c r="A25" s="22"/>
       <c r="B25" s="23"/>
       <c r="C25" s="21"/>
@@ -1190,7 +1165,7 @@
       <c r="H25" s="10"/>
       <c r="I25" s="9"/>
     </row>
-    <row r="26" spans="1:9" ht="17.3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
       <c r="A26" s="22"/>
       <c r="B26" s="23"/>
       <c r="C26" s="21"/>
@@ -1201,7 +1176,7 @@
       <c r="H26" s="10"/>
       <c r="I26" s="9"/>
     </row>
-    <row r="27" spans="1:9" ht="17.3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
       <c r="A27" s="22"/>
       <c r="B27" s="23"/>
       <c r="C27" s="21"/>
@@ -1212,7 +1187,7 @@
       <c r="H27" s="10"/>
       <c r="I27" s="9"/>
     </row>
-    <row r="28" spans="1:9" ht="17.3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
       <c r="A28" s="22"/>
       <c r="B28" s="23"/>
       <c r="C28" s="21"/>
@@ -1223,7 +1198,7 @@
       <c r="H28" s="10"/>
       <c r="I28" s="9"/>
     </row>
-    <row r="29" spans="1:9" ht="17.3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
       <c r="A29" s="22"/>
       <c r="B29" s="23"/>
       <c r="C29" s="21"/>
@@ -1234,7 +1209,7 @@
       <c r="H29" s="10"/>
       <c r="I29" s="9"/>
     </row>
-    <row r="30" spans="1:9" ht="17.3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
       <c r="A30" s="22"/>
       <c r="B30" s="23"/>
       <c r="C30" s="21"/>
@@ -1245,7 +1220,7 @@
       <c r="H30" s="10"/>
       <c r="I30" s="9"/>
     </row>
-    <row r="31" spans="1:9" ht="17.3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
       <c r="A31" s="22"/>
       <c r="B31" s="23"/>
       <c r="C31" s="21"/>
@@ -1256,7 +1231,7 @@
       <c r="H31" s="10"/>
       <c r="I31" s="9"/>
     </row>
-    <row r="32" spans="1:9" ht="17.3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
       <c r="A32" s="22"/>
       <c r="B32" s="23"/>
       <c r="C32" s="21"/>
@@ -1267,7 +1242,7 @@
       <c r="H32" s="10"/>
       <c r="I32" s="9"/>
     </row>
-    <row r="33" spans="1:9" ht="17.3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
       <c r="B33" s="7"/>
       <c r="C33" s="21"/>
@@ -1278,7 +1253,7 @@
       <c r="H33" s="10"/>
       <c r="I33" s="9"/>
     </row>
-    <row r="34" spans="1:9" ht="17.3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
       <c r="A34" s="6"/>
       <c r="B34" s="7"/>
       <c r="C34" s="21"/>
@@ -1289,7 +1264,7 @@
       <c r="H34" s="10"/>
       <c r="I34" s="9"/>
     </row>
-    <row r="35" spans="1:9" ht="17.850000000000001" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
         <v>11</v>
       </c>
@@ -1304,7 +1279,7 @@
       <c r="H35" s="10"/>
       <c r="I35" s="9"/>
     </row>
-    <row r="36" spans="1:9" ht="17.850000000000001" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="15"/>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
@@ -1546,15 +1521,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="75365404-5c48-41d8-865a-7f2026b82160" xsi:nil="true"/>
@@ -1563,6 +1529,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1585,14 +1560,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0BE1A59-8C13-4790-85C7-0C0527D61090}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14BBCEBA-3D86-4DE9-A442-C88237D1832E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1601,4 +1568,12 @@
     <ds:schemaRef ds:uri="0b767478-c6a5-46ac-ac91-475c6fa29b26"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0BE1A59-8C13-4790-85C7-0C0527D61090}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
ExcelMM_template table border bold
</commit_message>
<xml_diff>
--- a/GoodSunLMS/src/main/java/com/reality/util/excel/ExcelMM_template.xlsx
+++ b/GoodSunLMS/src/main/java/com/reality/util/excel/ExcelMM_template.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51CCC0A-694E-45F0-9F3C-5E6F7B695D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4FE123-ABB3-46B0-8E24-49E7190A479B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="230" yWindow="1110" windowWidth="14400" windowHeight="9430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3890" yWindow="1230" windowWidth="14400" windowHeight="9430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -249,21 +249,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -406,12 +391,33 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -422,7 +428,7 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -431,11 +437,11 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -444,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -455,13 +461,13 @@
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -470,83 +476,92 @@
     <xf numFmtId="179" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -854,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8438505C-A935-4586-A8B1-5DE40A2EF4C3}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I1:I1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -871,30 +886,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="27"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="30"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="23"/>
       <c r="G2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="31"/>
-      <c r="I2" s="32"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="25"/>
     </row>
     <row r="3" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -908,10 +923,10 @@
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="34"/>
+      <c r="B4" s="27"/>
       <c r="C4" s="12" t="s">
         <v>3</v>
       </c>
@@ -930,313 +945,313 @@
       <c r="H4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="17" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="9"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="30"/>
     </row>
     <row r="6" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="22"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="24"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="10"/>
       <c r="F6" s="8"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
       <c r="I6" s="9"/>
     </row>
     <row r="7" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="22"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="24"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="10"/>
       <c r="F7" s="8"/>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
       <c r="I7" s="9"/>
     </row>
     <row r="8" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="22"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="24"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="10"/>
       <c r="F8" s="8"/>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
       <c r="I8" s="9"/>
     </row>
     <row r="9" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="22"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="24"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="10"/>
       <c r="F9" s="8"/>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
       <c r="I9" s="9"/>
     </row>
     <row r="10" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="22"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="24"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="10"/>
       <c r="F10" s="8"/>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
       <c r="I10" s="9"/>
     </row>
     <row r="11" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="22"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="24"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="10"/>
       <c r="F11" s="8"/>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
       <c r="I11" s="9"/>
     </row>
     <row r="12" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="22"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="24"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="10"/>
       <c r="F12" s="8"/>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
       <c r="I12" s="9"/>
     </row>
     <row r="13" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="22"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="24"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="10"/>
       <c r="F13" s="8"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
       <c r="I13" s="9"/>
     </row>
     <row r="14" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="22"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="24"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="10"/>
       <c r="F14" s="8"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
       <c r="I14" s="9"/>
     </row>
     <row r="15" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="22"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="24"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="10"/>
       <c r="F15" s="8"/>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
       <c r="I15" s="9"/>
     </row>
     <row r="16" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="22"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="24"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="10"/>
       <c r="F16" s="8"/>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
       <c r="I16" s="9"/>
     </row>
     <row r="17" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="22"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="24"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="10"/>
       <c r="F17" s="8"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
       <c r="I17" s="9"/>
     </row>
     <row r="18" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="22"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="24"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="10"/>
       <c r="F18" s="8"/>
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
       <c r="I18" s="9"/>
     </row>
     <row r="19" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="22"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="24"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="10"/>
       <c r="F19" s="8"/>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
       <c r="I19" s="9"/>
     </row>
     <row r="20" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
-      <c r="A20" s="22"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="24"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="10"/>
       <c r="F20" s="8"/>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
       <c r="I20" s="9"/>
     </row>
     <row r="21" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="22"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="24"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="10"/>
       <c r="F21" s="8"/>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
       <c r="I21" s="9"/>
     </row>
     <row r="22" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
-      <c r="A22" s="22"/>
-      <c r="B22" s="23"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="24"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="10"/>
       <c r="F22" s="8"/>
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
       <c r="I22" s="9"/>
     </row>
     <row r="23" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
-      <c r="A23" s="22"/>
-      <c r="B23" s="23"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="24"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="10"/>
       <c r="F23" s="8"/>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
       <c r="I23" s="9"/>
     </row>
     <row r="24" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="22"/>
-      <c r="B24" s="23"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="24"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="10"/>
       <c r="F24" s="8"/>
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
       <c r="I24" s="9"/>
     </row>
     <row r="25" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
-      <c r="A25" s="22"/>
-      <c r="B25" s="23"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="24"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="10"/>
       <c r="F25" s="8"/>
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
       <c r="I25" s="9"/>
     </row>
     <row r="26" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
-      <c r="A26" s="22"/>
-      <c r="B26" s="23"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="24"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="10"/>
       <c r="F26" s="8"/>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
       <c r="I26" s="9"/>
     </row>
     <row r="27" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
-      <c r="A27" s="22"/>
-      <c r="B27" s="23"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="24"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="10"/>
       <c r="F27" s="8"/>
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
       <c r="I27" s="9"/>
     </row>
     <row r="28" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
-      <c r="A28" s="22"/>
-      <c r="B28" s="23"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="24"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="10"/>
       <c r="F28" s="8"/>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
       <c r="I28" s="9"/>
     </row>
     <row r="29" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
-      <c r="A29" s="22"/>
-      <c r="B29" s="23"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="24"/>
+      <c r="A29" s="6"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="10"/>
       <c r="F29" s="8"/>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
       <c r="I29" s="9"/>
     </row>
     <row r="30" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
-      <c r="A30" s="22"/>
-      <c r="B30" s="23"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="24"/>
+      <c r="A30" s="6"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="10"/>
       <c r="F30" s="8"/>
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
       <c r="I30" s="9"/>
     </row>
     <row r="31" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
-      <c r="A31" s="22"/>
-      <c r="B31" s="23"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="24"/>
+      <c r="A31" s="6"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="10"/>
       <c r="F31" s="8"/>
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
       <c r="I31" s="9"/>
     </row>
     <row r="32" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
-      <c r="A32" s="22"/>
-      <c r="B32" s="23"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="24"/>
+      <c r="A32" s="6"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="10"/>
       <c r="F32" s="8"/>
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
@@ -1245,8 +1260,8 @@
     <row r="33" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
       <c r="B33" s="7"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
       <c r="E33" s="10"/>
       <c r="F33" s="8"/>
       <c r="G33" s="10"/>
@@ -1256,8 +1271,8 @@
     <row r="34" spans="1:9" ht="17.5" x14ac:dyDescent="0.2">
       <c r="A34" s="6"/>
       <c r="B34" s="7"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
       <c r="E34" s="10"/>
       <c r="F34" s="8"/>
       <c r="G34" s="10"/>
@@ -1265,35 +1280,35 @@
       <c r="I34" s="9"/>
     </row>
     <row r="35" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="20" t="s">
+      <c r="B35" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
       <c r="E35" s="11"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="9"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="33"/>
     </row>
     <row r="36" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="17" t="s">
+      <c r="A36" s="34"/>
+      <c r="B36" s="35"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="F36" s="18">
+      <c r="F36" s="37">
         <f>SUM(F5:F35)</f>
         <v>0</v>
       </c>
-      <c r="G36" s="16"/>
-      <c r="H36" s="16"/>
-      <c r="I36" s="16"/>
+      <c r="G36" s="35"/>
+      <c r="H36" s="35"/>
+      <c r="I36" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1310,6 +1325,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="75365404-5c48-41d8-865a-7f2026b82160" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0b767478-c6a5-46ac-ac91-475c6fa29b26">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ドキュメント" ma:contentTypeID="0x0101000D8F77CBF0A2534F9509FAF6232E7B97" ma:contentTypeVersion="11" ma:contentTypeDescription="新しいドキュメントを作成します。" ma:contentTypeScope="" ma:versionID="b56741c68818c02055f012ce5e44eb4d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0b767478-c6a5-46ac-ac91-475c6fa29b26" xmlns:ns3="75365404-5c48-41d8-865a-7f2026b82160" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3797a4ed2471239fdb7af31dd85dd864" ns2:_="" ns3:_="">
     <xsd:import namespace="0b767478-c6a5-46ac-ac91-475c6fa29b26"/>
@@ -1520,27 +1555,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="75365404-5c48-41d8-865a-7f2026b82160" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0b767478-c6a5-46ac-ac91-475c6fa29b26">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0BE1A59-8C13-4790-85C7-0C0527D61090}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14BBCEBA-3D86-4DE9-A442-C88237D1832E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="75365404-5c48-41d8-865a-7f2026b82160"/>
+    <ds:schemaRef ds:uri="0b767478-c6a5-46ac-ac91-475c6fa29b26"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{268717EE-32EC-4B30-8359-609A165CCA38}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1557,23 +1591,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14BBCEBA-3D86-4DE9-A442-C88237D1832E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="75365404-5c48-41d8-865a-7f2026b82160"/>
-    <ds:schemaRef ds:uri="0b767478-c6a5-46ac-ac91-475c6fa29b26"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0BE1A59-8C13-4790-85C7-0C0527D61090}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>